<commit_message>
Runs 19-25 Logs & CRX
</commit_message>
<xml_diff>
--- a/DNAdilutionTemplate.xlsx
+++ b/DNAdilutionTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymond/Desktop/Frawgz/qPCR_Lab_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6050E314-1FEE-224E-AA73-9C05CBAD8295}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBB8888-DC82-3248-84B3-1922C434349C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11380" yWindow="460" windowWidth="12840" windowHeight="13360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14980" yWindow="460" windowWidth="14180" windowHeight="13360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet to Print From" sheetId="1" r:id="rId1"/>
@@ -6831,8 +6831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A743" workbookViewId="0">
-      <selection activeCell="A757" sqref="A757"/>
+    <sheetView tabSelected="1" topLeftCell="A858" workbookViewId="0">
+      <selection activeCell="A882" sqref="A882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>